<commit_message>
tests+newsletter subscription response fix
</commit_message>
<xml_diff>
--- a/backend tests.xlsx
+++ b/backend tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="241">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -757,6 +757,51 @@
   </si>
   <si>
     <t xml:space="preserve">T-51,T-52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/newsletter_subscription works (malformed request)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/newsletter_subscription/ with the body  „ {    "id": "&lt;b64encoded i” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 400 (BAD REQUEST), body: „{"status":"malformed_request","statuscode":"400"}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-55,T-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/newsletter_subscription works (duplicate user)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open postman 2. Send a request to  http://localhost:90/api/newsletter_subscription/ with the body  „ {   "email": "&lt;base64 encoded email&gt;",   "news_level": "&lt;base64 encoded string:2&gt;",   "language": "&lt;base64 encoded string:en&gt;"  }”  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 409 (CONFLICT), body: „{"status":"user_already_subscribed","statuscode":"409"}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 400 (BAD REQUEST), body: „{"status":"user_already_subscribed","statuscode":"409"}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-54,T-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if api/newsletter_subscription works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response: 200 (SUCCESS), body: „{     "status": "success",     "statuscode": "200" }"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-54,T-55</t>
   </si>
 </sst>
 </file>
@@ -901,7 +946,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -951,6 +996,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1203,10 +1252,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V60"/>
+  <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2952,6 +3001,93 @@
         <v>46074</v>
       </c>
     </row>
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I61" s="12" t="n">
+        <v>46079</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I62" s="12" t="n">
+        <v>46079</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I63" s="12" t="n">
+        <v>46079</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D50" r:id="rId1" display="1. Open postman 2. Send a request to  http://localhost:90/api/get_all_product_categories/ without a body or an auth header"/>

</xml_diff>